<commit_message>
added autocorr.do and other do file cleaning/work
</commit_message>
<xml_diff>
--- a/do_files/UKHLS_quants_output/coeff_tests_Q5_specEd.xlsx
+++ b/do_files/UKHLS_quants_output/coeff_tests_Q5_specEd.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="6">
   <si>
     <t>Chi2</t>
   </si>
@@ -93,7 +93,7 @@
       </c>
       <c r="B2"/>
       <c r="C2">
-        <v>8.1963511918633381e-015</v>
+        <v>1.0143979550127285e-009</v>
       </c>
     </row>
     <row r="3">
@@ -102,7 +102,7 @@
       </c>
       <c r="B3"/>
       <c r="C3">
-        <v>0.033042297363768562</v>
+        <v>0.094049108711074747</v>
       </c>
     </row>
     <row r="4">
@@ -111,7 +111,7 @@
       </c>
       <c r="B4"/>
       <c r="C4">
-        <v>0.019653276041281524</v>
+        <v>0.010859487766057534</v>
       </c>
     </row>
     <row r="5">
@@ -120,7 +120,7 @@
       </c>
       <c r="B5"/>
       <c r="C5">
-        <v>0.45440553942472295</v>
+        <v>0.62702728760089754</v>
       </c>
     </row>
   </sheetData>
@@ -146,7 +146,7 @@
       </c>
       <c r="B2"/>
       <c r="C2">
-        <v>0.25216859886786136</v>
+        <v>0.18534836829120924</v>
       </c>
     </row>
     <row r="3">
@@ -155,7 +155,7 @@
       </c>
       <c r="B3"/>
       <c r="C3">
-        <v>0.42262305040100434</v>
+        <v>0.65840609944649109</v>
       </c>
     </row>
     <row r="4">
@@ -164,7 +164,7 @@
       </c>
       <c r="B4"/>
       <c r="C4">
-        <v>0.046852739560310615</v>
+        <v>0.69861198658088808</v>
       </c>
     </row>
     <row r="5">
@@ -173,7 +173,7 @@
       </c>
       <c r="B5"/>
       <c r="C5">
-        <v>0.022647358700928856</v>
+        <v>0.70200611133569302</v>
       </c>
     </row>
   </sheetData>
@@ -199,7 +199,7 @@
       </c>
       <c r="B2"/>
       <c r="C2">
-        <v>0.19724964847302806</v>
+        <v>0.042232394403873698</v>
       </c>
     </row>
     <row r="3">
@@ -208,7 +208,7 @@
       </c>
       <c r="B3"/>
       <c r="C3">
-        <v>0.804483454185142</v>
+        <v>0.24541337938683686</v>
       </c>
     </row>
     <row r="4">
@@ -217,7 +217,7 @@
       </c>
       <c r="B4"/>
       <c r="C4">
-        <v>0.5805757379460954</v>
+        <v>0.80961077489224331</v>
       </c>
     </row>
     <row r="5">
@@ -226,7 +226,7 @@
       </c>
       <c r="B5"/>
       <c r="C5">
-        <v>0.24675520150724928</v>
+        <v>0.25996452292074584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before big find and replace on labor_income
</commit_message>
<xml_diff>
--- a/do_files/UKHLS_quants_output/coeff_tests_Q5_specEd.xlsx
+++ b/do_files/UKHLS_quants_output/coeff_tests_Q5_specEd.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="6">
   <si>
     <t>Chi2</t>
   </si>
@@ -93,7 +93,7 @@
       </c>
       <c r="B2"/>
       <c r="C2">
-        <v>1.0143979550127285e-009</v>
+        <v>4.6738344251187574e-009</v>
       </c>
     </row>
     <row r="3">
@@ -102,7 +102,7 @@
       </c>
       <c r="B3"/>
       <c r="C3">
-        <v>0.094049108711074747</v>
+        <v>0.079553397855037233</v>
       </c>
     </row>
     <row r="4">
@@ -111,7 +111,7 @@
       </c>
       <c r="B4"/>
       <c r="C4">
-        <v>0.010859487766057534</v>
+        <v>0.013483650518968333</v>
       </c>
     </row>
     <row r="5">
@@ -120,7 +120,7 @@
       </c>
       <c r="B5"/>
       <c r="C5">
-        <v>0.62702728760089754</v>
+        <v>0.72490962131736891</v>
       </c>
     </row>
   </sheetData>
@@ -146,7 +146,7 @@
       </c>
       <c r="B2"/>
       <c r="C2">
-        <v>0.18534836829120924</v>
+        <v>0.27885337384685355</v>
       </c>
     </row>
     <row r="3">
@@ -155,7 +155,7 @@
       </c>
       <c r="B3"/>
       <c r="C3">
-        <v>0.65840609944649109</v>
+        <v>0.43535181469514761</v>
       </c>
     </row>
     <row r="4">
@@ -164,7 +164,7 @@
       </c>
       <c r="B4"/>
       <c r="C4">
-        <v>0.69861198658088808</v>
+        <v>0.71183145149122529</v>
       </c>
     </row>
     <row r="5">
@@ -173,7 +173,7 @@
       </c>
       <c r="B5"/>
       <c r="C5">
-        <v>0.70200611133569302</v>
+        <v>0.63364478338084451</v>
       </c>
     </row>
   </sheetData>
@@ -199,7 +199,7 @@
       </c>
       <c r="B2"/>
       <c r="C2">
-        <v>0.042232394403873698</v>
+        <v>0.040766768295238391</v>
       </c>
     </row>
     <row r="3">
@@ -208,7 +208,7 @@
       </c>
       <c r="B3"/>
       <c r="C3">
-        <v>0.24541337938683686</v>
+        <v>0.22275970466618961</v>
       </c>
     </row>
     <row r="4">
@@ -217,7 +217,7 @@
       </c>
       <c r="B4"/>
       <c r="C4">
-        <v>0.80961077489224331</v>
+        <v>0.82767386520479658</v>
       </c>
     </row>
     <row r="5">
@@ -226,7 +226,7 @@
       </c>
       <c r="B5"/>
       <c r="C5">
-        <v>0.25996452292074584</v>
+        <v>0.28735577256720174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Looks like the replace and clean went well
</commit_message>
<xml_diff>
--- a/do_files/UKHLS_quants_output/coeff_tests_Q5_specEd.xlsx
+++ b/do_files/UKHLS_quants_output/coeff_tests_Q5_specEd.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="6">
   <si>
     <t>Chi2</t>
   </si>
@@ -93,7 +93,7 @@
       </c>
       <c r="B2"/>
       <c r="C2">
-        <v>4.6738344251187574e-009</v>
+        <v>4.6738344251231605e-009</v>
       </c>
     </row>
     <row r="3">
@@ -102,7 +102,7 @@
       </c>
       <c r="B3"/>
       <c r="C3">
-        <v>0.079553397855037233</v>
+        <v>0.079553397855026284</v>
       </c>
     </row>
     <row r="4">
@@ -111,7 +111,7 @@
       </c>
       <c r="B4"/>
       <c r="C4">
-        <v>0.013483650518968333</v>
+        <v>0.013483650518965511</v>
       </c>
     </row>
     <row r="5">
@@ -120,7 +120,7 @@
       </c>
       <c r="B5"/>
       <c r="C5">
-        <v>0.72490962131736891</v>
+        <v>0.72490962131729253</v>
       </c>
     </row>
   </sheetData>
@@ -146,7 +146,7 @@
       </c>
       <c r="B2"/>
       <c r="C2">
-        <v>0.27885337384685355</v>
+        <v>0.2788533738468737</v>
       </c>
     </row>
     <row r="3">
@@ -155,7 +155,7 @@
       </c>
       <c r="B3"/>
       <c r="C3">
-        <v>0.43535181469514761</v>
+        <v>0.43535181469511075</v>
       </c>
     </row>
     <row r="4">
@@ -164,7 +164,7 @@
       </c>
       <c r="B4"/>
       <c r="C4">
-        <v>0.71183145149122529</v>
+        <v>0.71183145149126625</v>
       </c>
     </row>
     <row r="5">
@@ -173,7 +173,7 @@
       </c>
       <c r="B5"/>
       <c r="C5">
-        <v>0.63364478338084451</v>
+        <v>0.63364478338084385</v>
       </c>
     </row>
   </sheetData>
@@ -199,7 +199,7 @@
       </c>
       <c r="B2"/>
       <c r="C2">
-        <v>0.040766768295238391</v>
+        <v>0.040766768295244359</v>
       </c>
     </row>
     <row r="3">
@@ -208,7 +208,7 @@
       </c>
       <c r="B3"/>
       <c r="C3">
-        <v>0.22275970466618961</v>
+        <v>0.22275970466613676</v>
       </c>
     </row>
     <row r="4">
@@ -217,7 +217,7 @@
       </c>
       <c r="B4"/>
       <c r="C4">
-        <v>0.82767386520479658</v>
+        <v>0.82767386520488773</v>
       </c>
     </row>
     <row r="5">
@@ -226,7 +226,7 @@
       </c>
       <c r="B5"/>
       <c r="C5">
-        <v>0.28735577256720174</v>
+        <v>0.28735577256720235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove employed but misisng labor earnings from data
</commit_message>
<xml_diff>
--- a/do_files/UKHLS_quants_output/coeff_tests_Q5_specEd.xlsx
+++ b/do_files/UKHLS_quants_output/coeff_tests_Q5_specEd.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="6">
   <si>
     <t>Chi2</t>
   </si>
@@ -93,7 +93,7 @@
       </c>
       <c r="B2"/>
       <c r="C2">
-        <v>4.6738344251231605e-009</v>
+        <v>1.9353399498926572e-008</v>
       </c>
     </row>
     <row r="3">
@@ -102,7 +102,7 @@
       </c>
       <c r="B3"/>
       <c r="C3">
-        <v>0.079553397855026284</v>
+        <v>0.052228098184643384</v>
       </c>
     </row>
     <row r="4">
@@ -111,7 +111,7 @@
       </c>
       <c r="B4"/>
       <c r="C4">
-        <v>0.013483650518965511</v>
+        <v>0.036294493198127067</v>
       </c>
     </row>
     <row r="5">
@@ -120,7 +120,7 @@
       </c>
       <c r="B5"/>
       <c r="C5">
-        <v>0.72490962131729253</v>
+        <v>0.27539661899984952</v>
       </c>
     </row>
   </sheetData>
@@ -146,7 +146,7 @@
       </c>
       <c r="B2"/>
       <c r="C2">
-        <v>0.2788533738468737</v>
+        <v>0.32646320078894442</v>
       </c>
     </row>
     <row r="3">
@@ -155,7 +155,7 @@
       </c>
       <c r="B3"/>
       <c r="C3">
-        <v>0.43535181469511075</v>
+        <v>0.7106859618415855</v>
       </c>
     </row>
     <row r="4">
@@ -164,7 +164,7 @@
       </c>
       <c r="B4"/>
       <c r="C4">
-        <v>0.71183145149126625</v>
+        <v>0.44057137274309721</v>
       </c>
     </row>
     <row r="5">
@@ -173,7 +173,7 @@
       </c>
       <c r="B5"/>
       <c r="C5">
-        <v>0.63364478338084385</v>
+        <v>0.49492243924521029</v>
       </c>
     </row>
   </sheetData>
@@ -199,7 +199,7 @@
       </c>
       <c r="B2"/>
       <c r="C2">
-        <v>0.040766768295244359</v>
+        <v>0.063293410790960958</v>
       </c>
     </row>
     <row r="3">
@@ -208,7 +208,7 @@
       </c>
       <c r="B3"/>
       <c r="C3">
-        <v>0.22275970466613676</v>
+        <v>0.47517390487835554</v>
       </c>
     </row>
     <row r="4">
@@ -217,7 +217,7 @@
       </c>
       <c r="B4"/>
       <c r="C4">
-        <v>0.82767386520488773</v>
+        <v>0.76995907575680145</v>
       </c>
     </row>
     <row r="5">
@@ -226,7 +226,7 @@
       </c>
       <c r="B5"/>
       <c r="C5">
-        <v>0.28735577256720235</v>
+        <v>0.32665046708725398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>